<commit_message>
1. Updated the Respondents import template.
</commit_message>
<xml_diff>
--- a/public/Templates/Respondents-Import-Template.xlsx
+++ b/public/Templates/Respondents-Import-Template.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t xml:space="preserve">r_id</t>
   </si>
@@ -118,22 +115,13 @@
     <t xml:space="preserve">ethnic_group</t>
   </si>
   <si>
+    <t xml:space="preserve">age_group </t>
+  </si>
+  <si>
     <t xml:space="preserve">employment_status</t>
   </si>
   <si>
-    <t xml:space="preserve">age_group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interview_date_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interview_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_downloaded_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Respondent Name</t>
+    <t xml:space="preserve">Respondent Seven</t>
   </si>
   <si>
     <t xml:space="preserve">BOMET</t>
@@ -148,7 +136,7 @@
     <t xml:space="preserve">Christian</t>
   </si>
   <si>
-    <t xml:space="preserve">Firstname Lastname</t>
+    <t xml:space="preserve">Respondent Eight</t>
   </si>
   <si>
     <t xml:space="preserve">MIGORI</t>
@@ -160,7 +148,7 @@
     <t xml:space="preserve">Moslem</t>
   </si>
   <si>
-    <t xml:space="preserve">Firstname Middlename Lastname</t>
+    <t xml:space="preserve">Respondent Nine</t>
   </si>
   <si>
     <t xml:space="preserve">KITUI</t>
@@ -214,6 +202,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -262,7 +251,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,6 +261,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,47 +285,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK4"/>
+  <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="8.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="1" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -425,119 +416,111 @@
       <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>70469</v>
+      </c>
       <c r="B2" s="0" t="n">
-        <v>70469</v>
+        <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>73234575</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>14553</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>712345678</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>14553</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>48373</v>
+      </c>
       <c r="B3" s="0" t="n">
-        <v>48373</v>
+        <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>712345678</v>
-      </c>
-      <c r="J3" s="0" t="n">
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>73345665</v>
+      </c>
+      <c r="I3" s="0" t="n">
         <v>65730</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="X3" s="0" t="s">
+      <c r="M3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="AC3" s="0" t="s">
-        <v>45</v>
+      <c r="W3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>51299</v>
+      </c>
       <c r="B4" s="0" t="n">
-        <v>51299</v>
+        <v>1</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>73356755</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>3728</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>723456789</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>3728</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="X4" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC4" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>